<commit_message>
house status update: 3 modes + API changes
</commit_message>
<xml_diff>
--- a/doc/UI APIs.xlsx
+++ b/doc/UI APIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/den/Shden/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E7D6F7-FD78-6A46-847E-C950891FB752}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC9FC4F-3DEA-2A41-9965-4F4D5C4015D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{3AFEF2B3-E87E-7B48-8F22-52B7E245566F}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{3AFEF2B3-E87E-7B48-8F22-52B7E245566F}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="64">
   <si>
     <t>Electricity</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>Shutters</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -269,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -382,6 +391,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -696,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931FF64E-E045-0B4E-8611-E8D9550376D4}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,9 +1060,10 @@
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="14" t="s">
         <v>53</v>
       </c>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -1061,10 +1075,10 @@
       <c r="C24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="15" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1234,6 +1248,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>